<commit_message>
clustering and heat mapping best variants across all Abs
</commit_message>
<xml_diff>
--- a/ab_data.xlsx
+++ b/ab_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1780" yWindow="0" windowWidth="23720" windowHeight="17340"/>
+    <workbookView xWindow="3820" yWindow="20" windowWidth="23720" windowHeight="17340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -848,9 +848,6 @@
     <t>D2-28</t>
   </si>
   <si>
-    <t>D2-2</t>
-  </si>
-  <si>
     <t>D3-03</t>
   </si>
   <si>
@@ -1167,6 +1164,9 @@
   </si>
   <si>
     <t>QVQLVQSGAEVKKPGSSVKVSCKASGGTFSSYAISWVRQAPGQGLEWMGGIIPIFGTANYAQKFQGRVTITADESTSTAYMELSSLRSEDTAVYYCARDGRGALQYWGQGTLVTVSS</t>
+  </si>
+  <si>
+    <t>D2-02</t>
   </si>
 </sst>
 </file>
@@ -2783,8 +2783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:S161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="D71" sqref="D71"/>
+    <sheetView tabSelected="1" topLeftCell="D33" workbookViewId="0">
+      <selection activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2810,34 +2810,34 @@
     <row r="4" spans="3:19" s="7" customFormat="1" ht="25" thickBot="1">
       <c r="C4" s="21"/>
       <c r="D4" s="8" t="s">
+        <v>339</v>
+      </c>
+      <c r="E4" s="9" t="s">
         <v>340</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="F4" s="8" t="s">
         <v>341</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="G4" s="22" t="s">
         <v>342</v>
-      </c>
-      <c r="G4" s="22" t="s">
-        <v>343</v>
       </c>
       <c r="H4" s="23" t="s">
         <v>118</v>
       </c>
       <c r="I4" s="9" t="s">
+        <v>343</v>
+      </c>
+      <c r="J4" s="8" t="s">
         <v>344</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="K4" s="22" t="s">
         <v>345</v>
       </c>
-      <c r="K4" s="22" t="s">
+      <c r="L4" s="23" t="s">
         <v>346</v>
       </c>
-      <c r="L4" s="23" t="s">
+      <c r="M4" s="22" t="s">
         <v>347</v>
-      </c>
-      <c r="M4" s="22" t="s">
-        <v>348</v>
       </c>
       <c r="N4" s="23" t="s">
         <v>247</v>
@@ -2849,10 +2849,10 @@
         <v>251</v>
       </c>
       <c r="Q4" s="23" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="R4" s="23" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="S4" s="21"/>
     </row>
@@ -2895,16 +2895,16 @@
         <v>236</v>
       </c>
       <c r="P5" s="13" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="Q5" s="26" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="R5" s="26" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="S5" s="25" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="6" spans="3:19">
@@ -2946,12 +2946,12 @@
         <v>236</v>
       </c>
       <c r="P6" s="13" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="Q6" s="26"/>
       <c r="R6" s="26"/>
       <c r="S6" s="25" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="7" spans="3:19">
@@ -2993,12 +2993,12 @@
         <v>237</v>
       </c>
       <c r="P7" s="13" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="Q7" s="26"/>
       <c r="R7" s="26"/>
       <c r="S7" s="25" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="8" spans="3:19">
@@ -3040,12 +3040,12 @@
         <v>236</v>
       </c>
       <c r="P8" s="13" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="Q8" s="25"/>
       <c r="R8" s="25"/>
       <c r="S8" s="27" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="9" spans="3:19">
@@ -3087,12 +3087,12 @@
         <v>236</v>
       </c>
       <c r="P9" s="13" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="Q9" s="25"/>
       <c r="R9" s="25"/>
       <c r="S9" s="27" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="10" spans="3:19">
@@ -3134,12 +3134,12 @@
         <v>238</v>
       </c>
       <c r="P10" s="13" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="Q10" s="25"/>
       <c r="R10" s="25"/>
       <c r="S10" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="11" spans="3:19">
@@ -3181,12 +3181,12 @@
         <v>238</v>
       </c>
       <c r="P11" s="13" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="Q11" s="25"/>
       <c r="R11" s="25"/>
       <c r="S11" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="12" spans="3:19">
@@ -3228,12 +3228,12 @@
         <v>238</v>
       </c>
       <c r="P12" s="13" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="Q12" s="25"/>
       <c r="R12" s="25"/>
       <c r="S12" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="13" spans="3:19">
@@ -3275,12 +3275,12 @@
         <v>238</v>
       </c>
       <c r="P13" s="13" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="Q13" s="25"/>
       <c r="R13" s="25"/>
       <c r="S13" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="14" spans="3:19">
@@ -3307,7 +3307,7 @@
         <v>148</v>
       </c>
       <c r="K14" s="13" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="L14" s="13">
         <v>21</v>
@@ -3322,12 +3322,12 @@
         <v>238</v>
       </c>
       <c r="P14" s="13" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="Q14" s="25"/>
       <c r="R14" s="25"/>
       <c r="S14" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="15" spans="3:19">
@@ -3369,12 +3369,12 @@
         <v>238</v>
       </c>
       <c r="P15" s="13" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="Q15" s="25"/>
       <c r="R15" s="25"/>
       <c r="S15" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="16" spans="3:19">
@@ -3401,7 +3401,7 @@
         <v>148</v>
       </c>
       <c r="K16" s="13" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="L16" s="13">
         <v>21</v>
@@ -3416,12 +3416,12 @@
         <v>238</v>
       </c>
       <c r="P16" s="13" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="Q16" s="25"/>
       <c r="R16" s="25"/>
       <c r="S16" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="17" spans="3:19">
@@ -3448,7 +3448,7 @@
         <v>149</v>
       </c>
       <c r="K17" s="13" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="L17" s="13">
         <v>8</v>
@@ -3463,12 +3463,12 @@
         <v>238</v>
       </c>
       <c r="P17" s="13" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="Q17" s="25"/>
       <c r="R17" s="25"/>
       <c r="S17" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="18" spans="3:19">
@@ -3486,7 +3486,7 @@
         <v>22</v>
       </c>
       <c r="H18" s="12" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="I18" s="12" t="s">
         <v>126</v>
@@ -3510,17 +3510,17 @@
         <v>238</v>
       </c>
       <c r="P18" s="13" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="Q18" s="25"/>
       <c r="R18" s="25"/>
       <c r="S18" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="19" spans="3:19">
       <c r="C19" s="25" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D19" s="30" t="s">
         <v>270</v>
@@ -3559,16 +3559,16 @@
         <v>238</v>
       </c>
       <c r="P19" s="13" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="Q19" s="26" t="s">
+        <v>375</v>
+      </c>
+      <c r="R19" s="13" t="s">
         <v>376</v>
       </c>
-      <c r="R19" s="13" t="s">
-        <v>377</v>
-      </c>
       <c r="S19" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="20" spans="3:19">
@@ -3610,12 +3610,12 @@
         <v>238</v>
       </c>
       <c r="P20" s="13" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="Q20" s="25"/>
       <c r="R20" s="25"/>
       <c r="S20" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="21" spans="3:19">
@@ -3657,18 +3657,18 @@
         <v>238</v>
       </c>
       <c r="P21" s="13" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="Q21" s="25"/>
       <c r="R21" s="25"/>
       <c r="S21" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="22" spans="3:19">
       <c r="C22" s="25"/>
       <c r="D22" s="11" t="s">
-        <v>275</v>
+        <v>381</v>
       </c>
       <c r="E22" s="12" t="s">
         <v>84</v>
@@ -3704,18 +3704,18 @@
         <v>238</v>
       </c>
       <c r="P22" s="13" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="Q22" s="25"/>
       <c r="R22" s="25"/>
       <c r="S22" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="23" spans="3:19">
       <c r="C23" s="25"/>
       <c r="D23" s="11" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E23" s="12" t="s">
         <v>85</v>
@@ -3751,18 +3751,18 @@
         <v>250</v>
       </c>
       <c r="P23" s="13" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="Q23" s="25"/>
       <c r="R23" s="25"/>
       <c r="S23" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="24" spans="3:19">
       <c r="C24" s="25"/>
       <c r="D24" s="11" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E24" s="12" t="s">
         <v>86</v>
@@ -3798,18 +3798,18 @@
         <v>250</v>
       </c>
       <c r="P24" s="13" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="Q24" s="25"/>
       <c r="R24" s="25"/>
       <c r="S24" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="25" spans="3:19">
       <c r="C25" s="25"/>
       <c r="D25" s="11" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E25" s="12" t="s">
         <v>86</v>
@@ -3845,18 +3845,18 @@
         <v>238</v>
       </c>
       <c r="P25" s="13" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="Q25" s="25"/>
       <c r="R25" s="25"/>
       <c r="S25" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="26" spans="3:19">
       <c r="C26" s="25"/>
       <c r="D26" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E26" s="12" t="s">
         <v>87</v>
@@ -3877,7 +3877,7 @@
         <v>149</v>
       </c>
       <c r="K26" s="13" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="L26" s="13">
         <v>8</v>
@@ -3892,18 +3892,18 @@
         <v>250</v>
       </c>
       <c r="P26" s="13" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="Q26" s="25"/>
       <c r="R26" s="25"/>
       <c r="S26" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="27" spans="3:19">
       <c r="C27" s="25"/>
       <c r="D27" s="11" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E27" s="12" t="s">
         <v>87</v>
@@ -3939,18 +3939,18 @@
         <v>238</v>
       </c>
       <c r="P27" s="13" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="Q27" s="25"/>
       <c r="R27" s="25"/>
       <c r="S27" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="28" spans="3:19">
       <c r="C28" s="25"/>
       <c r="D28" s="11" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E28" s="12" t="s">
         <v>86</v>
@@ -3986,18 +3986,18 @@
         <v>238</v>
       </c>
       <c r="P28" s="13" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="Q28" s="25"/>
       <c r="R28" s="25"/>
       <c r="S28" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="29" spans="3:19">
       <c r="C29" s="25"/>
       <c r="D29" s="11" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E29" s="12" t="s">
         <v>86</v>
@@ -4033,18 +4033,18 @@
         <v>250</v>
       </c>
       <c r="P29" s="13" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="Q29" s="25"/>
       <c r="R29" s="25"/>
       <c r="S29" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="30" spans="3:19">
       <c r="C30" s="25"/>
       <c r="D30" s="11" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E30" s="12" t="s">
         <v>88</v>
@@ -4065,7 +4065,7 @@
         <v>146</v>
       </c>
       <c r="K30" s="13" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="L30" s="13">
         <v>28</v>
@@ -4080,18 +4080,18 @@
         <v>238</v>
       </c>
       <c r="P30" s="13" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="Q30" s="25"/>
       <c r="R30" s="25"/>
       <c r="S30" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="31" spans="3:19">
       <c r="C31" s="25"/>
       <c r="D31" s="11" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E31" s="12" t="s">
         <v>89</v>
@@ -4127,18 +4127,18 @@
         <v>238</v>
       </c>
       <c r="P31" s="13" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="Q31" s="25"/>
       <c r="R31" s="25"/>
       <c r="S31" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="32" spans="3:19">
       <c r="C32" s="25"/>
       <c r="D32" s="11" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E32" s="12" t="s">
         <v>74</v>
@@ -4159,7 +4159,7 @@
         <v>146</v>
       </c>
       <c r="K32" s="13" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="L32" s="13">
         <v>15</v>
@@ -4174,18 +4174,18 @@
         <v>238</v>
       </c>
       <c r="P32" s="13" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="Q32" s="25"/>
       <c r="R32" s="25"/>
       <c r="S32" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="33" spans="3:19">
       <c r="C33" s="25"/>
       <c r="D33" s="11" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E33" s="12" t="s">
         <v>89</v>
@@ -4221,18 +4221,18 @@
         <v>250</v>
       </c>
       <c r="P33" s="13" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="Q33" s="25"/>
       <c r="R33" s="25"/>
       <c r="S33" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="34" spans="3:19">
       <c r="C34" s="25"/>
       <c r="D34" s="11" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E34" s="12" t="s">
         <v>90</v>
@@ -4268,18 +4268,18 @@
         <v>238</v>
       </c>
       <c r="P34" s="13" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="Q34" s="25"/>
       <c r="R34" s="25"/>
       <c r="S34" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="35" spans="3:19">
       <c r="C35" s="25"/>
       <c r="D35" s="11" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E35" s="12" t="s">
         <v>91</v>
@@ -4315,18 +4315,18 @@
         <v>250</v>
       </c>
       <c r="P35" s="13" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="Q35" s="25"/>
       <c r="R35" s="25"/>
       <c r="S35" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="36" spans="3:19">
       <c r="C36" s="25"/>
       <c r="D36" s="11" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E36" s="12" t="s">
         <v>106</v>
@@ -4362,18 +4362,18 @@
         <v>238</v>
       </c>
       <c r="P36" s="13" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="Q36" s="25"/>
       <c r="R36" s="25"/>
       <c r="S36" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="37" spans="3:19">
       <c r="C37" s="25"/>
       <c r="D37" s="11" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E37" s="12" t="s">
         <v>92</v>
@@ -4409,18 +4409,18 @@
         <v>250</v>
       </c>
       <c r="P37" s="13" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="Q37" s="25"/>
       <c r="R37" s="25"/>
       <c r="S37" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="38" spans="3:19">
       <c r="C38" s="25"/>
       <c r="D38" s="11" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E38" s="12" t="s">
         <v>93</v>
@@ -4456,18 +4456,18 @@
         <v>238</v>
       </c>
       <c r="P38" s="13" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="Q38" s="25"/>
       <c r="R38" s="25"/>
       <c r="S38" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="39" spans="3:19">
       <c r="C39" s="25"/>
       <c r="D39" s="11" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E39" s="12" t="s">
         <v>86</v>
@@ -4503,18 +4503,18 @@
         <v>238</v>
       </c>
       <c r="P39" s="13" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="Q39" s="25"/>
       <c r="R39" s="25"/>
       <c r="S39" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="40" spans="3:19">
       <c r="C40" s="25"/>
       <c r="D40" s="11" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E40" s="12" t="s">
         <v>94</v>
@@ -4555,13 +4555,13 @@
       <c r="Q40" s="25"/>
       <c r="R40" s="25"/>
       <c r="S40" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="41" spans="3:19">
       <c r="C41" s="25"/>
       <c r="D41" s="11" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E41" s="12" t="s">
         <v>94</v>
@@ -4597,18 +4597,18 @@
         <v>238</v>
       </c>
       <c r="P41" s="13" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="Q41" s="25"/>
       <c r="R41" s="25"/>
       <c r="S41" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="42" spans="3:19">
       <c r="C42" s="25"/>
       <c r="D42" s="11" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E42" s="12" t="s">
         <v>97</v>
@@ -4644,18 +4644,18 @@
         <v>240</v>
       </c>
       <c r="P42" s="13" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="Q42" s="25"/>
       <c r="R42" s="25"/>
       <c r="S42" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="43" spans="3:19">
       <c r="C43" s="25"/>
       <c r="D43" s="11" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E43" s="12" t="s">
         <v>95</v>
@@ -4691,18 +4691,18 @@
         <v>240</v>
       </c>
       <c r="P43" s="13" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="Q43" s="25"/>
       <c r="R43" s="25"/>
       <c r="S43" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="44" spans="3:19">
       <c r="C44" s="25"/>
       <c r="D44" s="11" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E44" s="12" t="s">
         <v>84</v>
@@ -4738,18 +4738,18 @@
         <v>240</v>
       </c>
       <c r="P44" s="13" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="Q44" s="25"/>
       <c r="R44" s="25"/>
       <c r="S44" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="45" spans="3:19">
       <c r="C45" s="25"/>
       <c r="D45" s="11" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E45" s="12" t="s">
         <v>96</v>
@@ -4770,7 +4770,7 @@
         <v>150</v>
       </c>
       <c r="K45" s="13" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="L45" s="13">
         <v>14</v>
@@ -4785,18 +4785,18 @@
         <v>240</v>
       </c>
       <c r="P45" s="13" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="Q45" s="25"/>
       <c r="R45" s="25"/>
       <c r="S45" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="46" spans="3:19">
       <c r="C46" s="25"/>
       <c r="D46" s="11" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E46" s="12" t="s">
         <v>94</v>
@@ -4832,18 +4832,18 @@
         <v>240</v>
       </c>
       <c r="P46" s="13" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="Q46" s="25"/>
       <c r="R46" s="25"/>
       <c r="S46" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="47" spans="3:19">
       <c r="C47" s="25"/>
       <c r="D47" s="11" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E47" s="12" t="s">
         <v>95</v>
@@ -4879,18 +4879,18 @@
         <v>240</v>
       </c>
       <c r="P47" s="13" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="Q47" s="25"/>
       <c r="R47" s="25"/>
       <c r="S47" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="48" spans="3:19">
       <c r="C48" s="25"/>
       <c r="D48" s="11" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E48" s="12" t="s">
         <v>98</v>
@@ -4926,18 +4926,18 @@
         <v>240</v>
       </c>
       <c r="P48" s="13" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="Q48" s="25"/>
       <c r="R48" s="25"/>
       <c r="S48" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="49" spans="3:19">
       <c r="C49" s="25"/>
       <c r="D49" s="11" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E49" s="12" t="s">
         <v>83</v>
@@ -4958,7 +4958,7 @@
         <v>147</v>
       </c>
       <c r="K49" s="13" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="L49" s="13">
         <v>22</v>
@@ -4973,18 +4973,18 @@
         <v>240</v>
       </c>
       <c r="P49" s="13" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="Q49" s="25"/>
       <c r="R49" s="25"/>
       <c r="S49" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="50" spans="3:19">
       <c r="C50" s="25"/>
       <c r="D50" s="11" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E50" s="12" t="s">
         <v>99</v>
@@ -5020,18 +5020,18 @@
         <v>225</v>
       </c>
       <c r="P50" s="13" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="Q50" s="25"/>
       <c r="R50" s="25"/>
       <c r="S50" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="51" spans="3:19">
       <c r="C51" s="25"/>
       <c r="D51" s="11" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E51" s="12" t="s">
         <v>94</v>
@@ -5067,18 +5067,18 @@
         <v>241</v>
       </c>
       <c r="P51" s="13" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="Q51" s="25"/>
       <c r="R51" s="25"/>
       <c r="S51" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="52" spans="3:19">
       <c r="C52" s="25"/>
       <c r="D52" s="11" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E52" s="12" t="s">
         <v>102</v>
@@ -5114,18 +5114,18 @@
         <v>241</v>
       </c>
       <c r="P52" s="13" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="Q52" s="25"/>
       <c r="R52" s="25"/>
       <c r="S52" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="53" spans="3:19">
       <c r="C53" s="25"/>
       <c r="D53" s="11" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E53" s="12" t="s">
         <v>94</v>
@@ -5161,20 +5161,20 @@
         <v>241</v>
       </c>
       <c r="P53" s="13" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="Q53" s="25"/>
       <c r="R53" s="25"/>
       <c r="S53" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="54" spans="3:19">
       <c r="C54" s="25" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D54" s="30" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E54" s="12" t="s">
         <v>102</v>
@@ -5210,22 +5210,22 @@
         <v>241</v>
       </c>
       <c r="P54" s="13" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="Q54" s="32" t="s">
+        <v>377</v>
+      </c>
+      <c r="R54" s="32" t="s">
         <v>378</v>
       </c>
-      <c r="R54" s="32" t="s">
-        <v>379</v>
-      </c>
       <c r="S54" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="55" spans="3:19">
       <c r="C55" s="25"/>
       <c r="D55" s="11" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E55" s="12" t="s">
         <v>94</v>
@@ -5246,7 +5246,7 @@
         <v>149</v>
       </c>
       <c r="K55" s="13" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="L55" s="13">
         <v>12</v>
@@ -5261,18 +5261,18 @@
         <v>241</v>
       </c>
       <c r="P55" s="13" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="Q55" s="25"/>
       <c r="R55" s="25"/>
       <c r="S55" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="56" spans="3:19">
       <c r="C56" s="25"/>
       <c r="D56" s="11" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E56" s="12" t="s">
         <v>94</v>
@@ -5293,7 +5293,7 @@
         <v>148</v>
       </c>
       <c r="K56" s="13" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="L56" s="13">
         <v>9</v>
@@ -5308,18 +5308,18 @@
         <v>241</v>
       </c>
       <c r="P56" s="13" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="Q56" s="25"/>
       <c r="R56" s="25"/>
       <c r="S56" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="57" spans="3:19">
       <c r="C57" s="25"/>
       <c r="D57" s="11" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E57" s="12" t="s">
         <v>94</v>
@@ -5340,7 +5340,7 @@
         <v>149</v>
       </c>
       <c r="K57" s="13" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="L57" s="13">
         <v>11</v>
@@ -5355,18 +5355,18 @@
         <v>241</v>
       </c>
       <c r="P57" s="13" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="Q57" s="25"/>
       <c r="R57" s="25"/>
       <c r="S57" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="58" spans="3:19">
       <c r="C58" s="25"/>
       <c r="D58" s="11" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E58" s="12" t="s">
         <v>94</v>
@@ -5387,7 +5387,7 @@
         <v>146</v>
       </c>
       <c r="K58" s="13" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="L58" s="13">
         <v>17</v>
@@ -5402,18 +5402,18 @@
         <v>241</v>
       </c>
       <c r="P58" s="13" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="Q58" s="25"/>
       <c r="R58" s="25"/>
       <c r="S58" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="59" spans="3:19">
       <c r="C59" s="25"/>
       <c r="D59" s="11" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E59" s="12" t="s">
         <v>94</v>
@@ -5434,7 +5434,7 @@
         <v>146</v>
       </c>
       <c r="K59" s="13" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="L59" s="13">
         <v>21</v>
@@ -5449,20 +5449,20 @@
         <v>241</v>
       </c>
       <c r="P59" s="13" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="Q59" s="25"/>
       <c r="R59" s="25"/>
       <c r="S59" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="60" spans="3:19">
       <c r="C60" s="25" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D60" s="30" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E60" s="12" t="s">
         <v>94</v>
@@ -5498,22 +5498,22 @@
         <v>241</v>
       </c>
       <c r="P60" s="13" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="Q60" s="33" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="R60" s="25" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="S60" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="61" spans="3:19">
       <c r="C61" s="25"/>
       <c r="D61" s="11" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E61" s="12" t="s">
         <v>94</v>
@@ -5549,18 +5549,18 @@
         <v>241</v>
       </c>
       <c r="P61" s="13" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="Q61" s="25"/>
       <c r="R61" s="25"/>
       <c r="S61" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="62" spans="3:19">
       <c r="C62" s="25"/>
       <c r="D62" s="11" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E62" s="12" t="s">
         <v>89</v>
@@ -5596,18 +5596,18 @@
         <v>241</v>
       </c>
       <c r="P62" s="13" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="Q62" s="25"/>
       <c r="R62" s="25"/>
       <c r="S62" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="63" spans="3:19">
       <c r="C63" s="25"/>
       <c r="D63" s="11" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E63" s="12" t="s">
         <v>76</v>
@@ -5628,7 +5628,7 @@
         <v>147</v>
       </c>
       <c r="K63" s="13" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="L63" s="13">
         <v>19</v>
@@ -5643,18 +5643,18 @@
         <v>241</v>
       </c>
       <c r="P63" s="13" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="Q63" s="25"/>
       <c r="R63" s="25"/>
       <c r="S63" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="64" spans="3:19">
       <c r="C64" s="25"/>
       <c r="D64" s="11" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E64" s="12" t="s">
         <v>103</v>
@@ -5690,18 +5690,18 @@
         <v>241</v>
       </c>
       <c r="P64" s="13" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="Q64" s="25"/>
       <c r="R64" s="25"/>
       <c r="S64" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="65" spans="3:19">
       <c r="C65" s="25"/>
       <c r="D65" s="11" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E65" s="12" t="s">
         <v>104</v>
@@ -5737,18 +5737,18 @@
         <v>241</v>
       </c>
       <c r="P65" s="13" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="Q65" s="25"/>
       <c r="R65" s="25"/>
       <c r="S65" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="66" spans="3:19">
       <c r="C66" s="25"/>
       <c r="D66" s="11" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E66" s="12" t="s">
         <v>79</v>
@@ -5784,18 +5784,18 @@
         <v>242</v>
       </c>
       <c r="P66" s="13" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="Q66" s="25"/>
       <c r="R66" s="25"/>
       <c r="S66" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="67" spans="3:19">
       <c r="C67" s="25"/>
       <c r="D67" s="11" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E67" s="12" t="s">
         <v>78</v>
@@ -5831,18 +5831,18 @@
         <v>244</v>
       </c>
       <c r="P67" s="13" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="Q67" s="25"/>
       <c r="R67" s="25"/>
       <c r="S67" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="68" spans="3:19">
       <c r="C68" s="25"/>
       <c r="D68" s="11" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E68" s="12" t="s">
         <v>94</v>
@@ -5878,18 +5878,18 @@
         <v>244</v>
       </c>
       <c r="P68" s="13" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="Q68" s="25"/>
       <c r="R68" s="25"/>
       <c r="S68" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="69" spans="3:19">
       <c r="C69" s="25"/>
       <c r="D69" s="11" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E69" s="12" t="s">
         <v>105</v>
@@ -5910,7 +5910,7 @@
         <v>147</v>
       </c>
       <c r="K69" s="13" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="L69" s="13">
         <v>18</v>
@@ -5925,18 +5925,18 @@
         <v>244</v>
       </c>
       <c r="P69" s="13" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="Q69" s="25"/>
       <c r="R69" s="25"/>
       <c r="S69" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="70" spans="3:19">
       <c r="C70" s="25"/>
       <c r="D70" s="11" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E70" s="12" t="s">
         <v>78</v>
@@ -5972,18 +5972,18 @@
         <v>244</v>
       </c>
       <c r="P70" s="13" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="Q70" s="25"/>
       <c r="R70" s="25"/>
       <c r="S70" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="71" spans="3:19">
       <c r="C71" s="25"/>
       <c r="D71" s="11" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E71" s="12" t="s">
         <v>82</v>
@@ -6024,13 +6024,13 @@
       <c r="Q71" s="25"/>
       <c r="R71" s="25"/>
       <c r="S71" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="72" spans="3:19">
       <c r="C72" s="25"/>
       <c r="D72" s="11" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E72" s="12" t="s">
         <v>87</v>
@@ -6051,7 +6051,7 @@
         <v>146</v>
       </c>
       <c r="K72" s="13" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="L72" s="13">
         <v>24</v>
@@ -6066,18 +6066,18 @@
         <v>244</v>
       </c>
       <c r="P72" s="13" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="Q72" s="25"/>
       <c r="R72" s="25"/>
       <c r="S72" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="73" spans="3:19">
       <c r="C73" s="25"/>
       <c r="D73" s="11" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E73" s="12" t="s">
         <v>79</v>
@@ -6113,18 +6113,18 @@
         <v>241</v>
       </c>
       <c r="P73" s="13" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="Q73" s="25"/>
       <c r="R73" s="25"/>
       <c r="S73" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="74" spans="3:19">
       <c r="C74" s="25"/>
       <c r="D74" s="11" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E74" s="12" t="s">
         <v>80</v>
@@ -6160,18 +6160,18 @@
         <v>225</v>
       </c>
       <c r="P74" s="13" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="Q74" s="25"/>
       <c r="R74" s="25"/>
       <c r="S74" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="75" spans="3:19">
       <c r="C75" s="25"/>
       <c r="D75" s="11" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E75" s="12" t="s">
         <v>86</v>
@@ -6207,18 +6207,18 @@
         <v>240</v>
       </c>
       <c r="P75" s="13" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="Q75" s="25"/>
       <c r="R75" s="25"/>
       <c r="S75" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="76" spans="3:19">
       <c r="C76" s="25"/>
       <c r="D76" s="11" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E76" s="12" t="s">
         <v>76</v>
@@ -6254,18 +6254,18 @@
         <v>236</v>
       </c>
       <c r="P76" s="13" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="Q76" s="25"/>
       <c r="R76" s="25"/>
       <c r="S76" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="77" spans="3:19">
       <c r="C77" s="25"/>
       <c r="D77" s="11" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E77" s="12" t="s">
         <v>100</v>
@@ -6301,18 +6301,18 @@
         <v>236</v>
       </c>
       <c r="P77" s="13" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="Q77" s="25"/>
       <c r="R77" s="25"/>
       <c r="S77" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="78" spans="3:19">
       <c r="C78" s="25"/>
       <c r="D78" s="11" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E78" s="12" t="s">
         <v>101</v>
@@ -6348,18 +6348,18 @@
         <v>243</v>
       </c>
       <c r="P78" s="13" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="Q78" s="25"/>
       <c r="R78" s="25"/>
       <c r="S78" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="79" spans="3:19">
       <c r="C79" s="25"/>
       <c r="D79" s="11" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E79" s="12" t="s">
         <v>77</v>
@@ -6395,12 +6395,12 @@
         <v>213</v>
       </c>
       <c r="P79" s="13" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="Q79" s="25"/>
       <c r="R79" s="25"/>
       <c r="S79" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="80" spans="3:19">
@@ -6453,7 +6453,7 @@
     </row>
     <row r="83" spans="4:19">
       <c r="D83" s="19" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E83" s="18"/>
       <c r="F83" s="16"/>
@@ -6470,7 +6470,7 @@
     </row>
     <row r="84" spans="4:19">
       <c r="D84" s="19" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E84" s="1"/>
       <c r="F84" s="16"/>
@@ -6487,7 +6487,7 @@
     </row>
     <row r="85" spans="4:19">
       <c r="D85" s="19" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E85" s="20"/>
       <c r="F85" s="16"/>
@@ -6504,7 +6504,7 @@
     </row>
     <row r="86" spans="4:19">
       <c r="D86" s="19" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E86" s="1"/>
       <c r="F86" s="16"/>
@@ -6538,7 +6538,7 @@
     </row>
     <row r="88" spans="4:19">
       <c r="D88" s="19" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E88" s="1"/>
       <c r="F88" s="16"/>

</xml_diff>